<commit_message>
Added SDGs research note
</commit_message>
<xml_diff>
--- a/research-notes/01-WaterAndDrought.xlsx
+++ b/research-notes/01-WaterAndDrought.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17780" yWindow="460" windowWidth="14360" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8100" yWindow="1280" windowWidth="14360" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Humidity provinces</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Forest cover (Ha)</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -85,7 +88,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,6 +111,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -126,9 +145,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -136,8 +161,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="8">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,9 +614,8 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>100</v>
+      <c r="F10" t="s">
+        <v>16</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -605,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>